<commit_message>
atualizando os artefatos para a AC5 de engenharia de requisitos
</commit_message>
<xml_diff>
--- a/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cd3af5bce398e7e/ADS/terceiroSemestre/engenharia_de_requisitos/ACS/AC4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cd3af5bce398e7e/ADS/terceiroSemestre/engenharia_de_requisitos/ACS/AC5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{E39E42E0-5A65-4F2C-A57E-E39DBDEE4A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{096DB1A3-191A-4FDE-BB22-D01016F89D0D}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{E39E42E0-5A65-4F2C-A57E-E39DBDEE4A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0DFDAD1-1EB4-4C17-BF00-10054646B430}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7B33A48A-E70E-4377-8D1B-5BACB7F573AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7B33A48A-E70E-4377-8D1B-5BACB7F573AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Externo</t>
   </si>
@@ -151,6 +151,33 @@
   </si>
   <si>
     <t>Carregamento do veículo com produtos</t>
+  </si>
+  <si>
+    <t>Tratar troca de produto</t>
+  </si>
+  <si>
+    <t>Cliente faz pedido de troca</t>
+  </si>
+  <si>
+    <t>Cliente recebe um novo produto do mesmo tipo</t>
+  </si>
+  <si>
+    <t>Produto defeituoso é enviado para o almoxarifado</t>
+  </si>
+  <si>
+    <t>Funcionário verifica mau uso do produto ou não encontra falhas</t>
+  </si>
+  <si>
+    <t>X(16)</t>
+  </si>
+  <si>
+    <t>X(17)</t>
+  </si>
+  <si>
+    <t>X(18)</t>
+  </si>
+  <si>
+    <t>A garantia e o produto são avaliados</t>
   </si>
 </sst>
 </file>
@@ -174,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +244,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -381,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -429,6 +468,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -441,24 +498,54 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -477,17 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -807,7 +884,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,22 +900,22 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
     </row>
     <row r="2" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
@@ -865,11 +942,11 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="36" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="11">
@@ -888,9 +965,9 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="11">
         <v>2</v>
       </c>
@@ -907,9 +984,9 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="11">
         <v>3</v>
       </c>
@@ -926,9 +1003,9 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="25" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="36" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="11">
@@ -947,9 +1024,9 @@
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="11">
         <v>5</v>
       </c>
@@ -966,9 +1043,9 @@
       <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="11">
         <v>6</v>
       </c>
@@ -985,9 +1062,9 @@
       <c r="L8" s="15"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="27"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="11">
         <v>7</v>
       </c>
@@ -1003,11 +1080,11 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="36" t="s">
         <v>15</v>
       </c>
@@ -1027,9 +1104,9 @@
       <c r="L10" s="15"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="11">
         <v>9</v>
       </c>
@@ -1046,9 +1123,9 @@
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="11">
         <v>10</v>
       </c>
@@ -1065,9 +1142,9 @@
       <c r="L12" s="15"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="37"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="11">
         <v>11</v>
       </c>
@@ -1084,9 +1161,9 @@
       <c r="L13" s="15"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="38"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="11">
         <v>12</v>
       </c>
@@ -1102,9 +1179,9 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="36" t="s">
         <v>20</v>
       </c>
@@ -1124,9 +1201,9 @@
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="11">
         <v>14</v>
       </c>
@@ -1143,9 +1220,9 @@
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="38"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="17">
         <v>15</v>
       </c>
@@ -1162,31 +1239,145 @@
       <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="12"/>
+      <c r="B18" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="17">
+        <v>16</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="12"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="17">
+        <v>17</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E20" s="12"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="17">
+        <v>18</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="12"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="19">
+        <v>19</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="15"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="12"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="35">
+        <v>20</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E23" s="12"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E24" s="12"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E25" s="12"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E26" s="12"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E27" s="12"/>
@@ -1237,7 +1428,7 @@
       <c r="E42" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="20">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:C9"/>
     <mergeCell ref="I1:K1"/>
@@ -1245,6 +1436,19 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="B10:C17"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B18:C23"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>